<commit_message>
v4 power layout is almost done, rst and a 3v3 line is left to be routed and then DRC
</commit_message>
<xml_diff>
--- a/HYDRA_V4_POWER/STM32G473RET6_PINOUT.xlsx
+++ b/HYDRA_V4_POWER/STM32G473RET6_PINOUT.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\se097192\Documents\0_PERSONAL\HYDRA\HYDRA_V4_LINK\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\se097192\Documents\0_PERSONAL\HYDRA\HYDRA_V4_POWER\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE6ABD84-5251-4941-8C3A-8282945E9282}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04370D79-7979-4F57-9489-FDE56ADEFD8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="588" yWindow="384" windowWidth="17280" windowHeight="10044" xr2:uid="{6B9885FF-AF60-4EEC-BBBC-D143F7D9FDBE}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6B9885FF-AF60-4EEC-BBBC-D143F7D9FDBE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="128">
   <si>
     <t>SPI</t>
   </si>
@@ -308,109 +308,118 @@
     <t>PB9</t>
   </si>
   <si>
-    <t>HYDRA_V3_LINK</t>
-  </si>
-  <si>
-    <t>ETH_NSS</t>
-  </si>
-  <si>
-    <t>ETH_SCLK</t>
-  </si>
-  <si>
-    <t>ETH_MISO</t>
-  </si>
-  <si>
-    <t>ETH_MOSI</t>
-  </si>
-  <si>
-    <t>ETH_NRST</t>
-  </si>
-  <si>
-    <t>ETH_NINT</t>
-  </si>
-  <si>
-    <t>RFD TX</t>
-  </si>
-  <si>
-    <t>RFD RX</t>
-  </si>
-  <si>
-    <t>CAN0_RX</t>
-  </si>
-  <si>
-    <t>CAN0_TX</t>
-  </si>
-  <si>
     <t>TCAN1146_nCS</t>
   </si>
   <si>
-    <t>CAN1_RX</t>
-  </si>
-  <si>
-    <t>CAN1_TX</t>
-  </si>
-  <si>
-    <t>SD_nCS</t>
-  </si>
-  <si>
-    <t>SD_SCLK</t>
-  </si>
-  <si>
-    <t>SD_MISO</t>
-  </si>
-  <si>
-    <t>SD_MOSI</t>
-  </si>
-  <si>
-    <t>SD_nCD</t>
-  </si>
-  <si>
-    <t>LORA_nCS</t>
-  </si>
-  <si>
-    <t>HYDRA_5V_V_SENSE</t>
-  </si>
-  <si>
-    <t>HYDRA_5V_I_SENSE</t>
-  </si>
-  <si>
-    <t>PYRO_PWR_V_SENSE</t>
-  </si>
-  <si>
     <t>SERCOM I/O</t>
   </si>
   <si>
     <t>ANALOG I/O</t>
   </si>
   <si>
-    <t>PYRO_PWR_I_SENSE</t>
-  </si>
-  <si>
-    <t>HYDRA_3V3_V_SENSE</t>
-  </si>
-  <si>
-    <t>HYDRA_3V3_I_SENSE</t>
-  </si>
-  <si>
-    <t>VCC_V_SENSE</t>
+    <t>HYDRA_V4_POWER</t>
+  </si>
+  <si>
+    <t>TCAN1146_SCLK</t>
+  </si>
+  <si>
+    <t>TCAN1146_MISO</t>
+  </si>
+  <si>
+    <t>TCAN1146_MOSI</t>
+  </si>
+  <si>
+    <t>TCAN1146_RX</t>
+  </si>
+  <si>
+    <t>TCAN1146_TX</t>
+  </si>
+  <si>
+    <t>TCAN330_RX</t>
+  </si>
+  <si>
+    <t>TCAN330_TX</t>
+  </si>
+  <si>
+    <t>LS_IMON_2</t>
+  </si>
+  <si>
+    <t>LS_IMON_1</t>
+  </si>
+  <si>
+    <t>LS_IMON_0</t>
+  </si>
+  <si>
+    <t>LS_PG_2</t>
+  </si>
+  <si>
+    <t>LS_PG_1</t>
+  </si>
+  <si>
+    <t>LS_PG_0</t>
+  </si>
+  <si>
+    <t>ADC_nCS</t>
   </si>
   <si>
     <t>INT_3V3_V_SENSE</t>
   </si>
   <si>
-    <t>OUTPUT_V_SENSE</t>
-  </si>
-  <si>
-    <t>VBAT_V_SENSE</t>
-  </si>
-  <si>
-    <t>LORA_nRST</t>
-  </si>
-  <si>
-    <t>BAT_I_SENSE</t>
-  </si>
-  <si>
-    <t>TBC (RFD900)</t>
+    <t>INT_VCC_V_SENSE</t>
+  </si>
+  <si>
+    <t>3V3_EN</t>
+  </si>
+  <si>
+    <t>5V_EN</t>
+  </si>
+  <si>
+    <t>STAT_nPG</t>
+  </si>
+  <si>
+    <t>5V_V_SENSE</t>
+  </si>
+  <si>
+    <t>3V3_V_SENSE</t>
+  </si>
+  <si>
+    <t>M1_INH</t>
+  </si>
+  <si>
+    <t>M2_INH</t>
+  </si>
+  <si>
+    <t>M3_INH</t>
+  </si>
+  <si>
+    <t>M1_I_SENSE</t>
+  </si>
+  <si>
+    <t>M1_V_SENSE</t>
+  </si>
+  <si>
+    <t>M2_I_SENSE</t>
+  </si>
+  <si>
+    <t>M2_V_SENSE</t>
+  </si>
+  <si>
+    <t>M3_I_SENSE</t>
+  </si>
+  <si>
+    <t>ADC_nRST</t>
+  </si>
+  <si>
+    <t>CUR_TRIP_RST</t>
+  </si>
+  <si>
+    <t>M1_OC_FAULT</t>
+  </si>
+  <si>
+    <t>MCU_R_LED</t>
+  </si>
+  <si>
+    <t>MCU_G_LED</t>
   </si>
 </sst>
 </file>
@@ -464,7 +473,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -806,8 +815,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71B6B797-796C-44D6-BE9C-10AF3EFF403F}">
   <dimension ref="A1:L49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="L39" sqref="L39"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="L11" sqref="C11:L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -827,7 +836,7 @@
   <sheetData>
     <row r="1" spans="1:12" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="J1" s="6" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="K1" s="6"/>
       <c r="L1" s="6"/>
@@ -858,710 +867,800 @@
         <v>14</v>
       </c>
       <c r="J2" t="s">
-        <v>113</v>
+        <v>91</v>
       </c>
       <c r="K2" t="s">
-        <v>114</v>
+        <v>92</v>
       </c>
       <c r="L2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A3">
+      <c r="A3" s="4">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="H3">
-        <v>5</v>
-      </c>
-      <c r="J3" t="s">
+      <c r="B3" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H3" s="4">
+        <v>5</v>
+      </c>
+      <c r="K3" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>8</v>
-      </c>
-      <c r="B4" t="s">
+      <c r="A4" s="4">
+        <v>8</v>
+      </c>
+      <c r="B4" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D4" t="s">
+      <c r="C4" s="4"/>
+      <c r="D4" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="F4" t="s">
-        <v>8</v>
-      </c>
-      <c r="G4" t="s">
-        <v>8</v>
-      </c>
-      <c r="H4">
+      <c r="E4" s="4"/>
+      <c r="F4" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H4" s="4">
         <v>5</v>
       </c>
       <c r="K4" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A5">
+      <c r="A5" s="4">
         <v>9</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D5" t="s">
+      <c r="C5" s="4"/>
+      <c r="D5" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F5" t="s">
-        <v>8</v>
-      </c>
-      <c r="G5" t="s">
-        <v>8</v>
-      </c>
-      <c r="H5">
+      <c r="E5" s="4"/>
+      <c r="F5" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H5" s="4">
         <v>3.6</v>
       </c>
-      <c r="K5" t="s">
-        <v>111</v>
+      <c r="K5" s="4" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A6">
+      <c r="A6" s="4">
         <v>10</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="F6" t="s">
-        <v>8</v>
-      </c>
-      <c r="G6" t="s">
-        <v>8</v>
-      </c>
-      <c r="H6">
-        <v>5</v>
-      </c>
-      <c r="K6" t="s">
-        <v>120</v>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H6" s="4">
+        <v>5</v>
+      </c>
+      <c r="K6" s="4" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A7">
+      <c r="A7" s="4">
         <v>11</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="F7" t="s">
-        <v>8</v>
-      </c>
-      <c r="G7" t="s">
-        <v>8</v>
-      </c>
-      <c r="H7">
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H7" s="4">
         <v>3.6</v>
       </c>
-      <c r="K7" t="s">
-        <v>110</v>
+      <c r="K7" s="4" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A8">
+      <c r="A8" s="4">
         <v>12</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="F8" t="s">
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4" t="s">
         <v>8</v>
       </c>
       <c r="G8" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="H8">
+      <c r="H8" s="4">
         <v>3.6</v>
       </c>
-      <c r="K8" t="s">
+      <c r="K8" s="4" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A9">
+      <c r="A9" s="4">
         <v>13</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="F9" t="s">
-        <v>8</v>
-      </c>
-      <c r="G9" t="s">
-        <v>8</v>
-      </c>
-      <c r="H9">
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H9" s="4">
         <v>3.6</v>
       </c>
-      <c r="K9" t="s">
-        <v>116</v>
+      <c r="K9" s="4" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A10">
+      <c r="A10" s="4">
         <v>14</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D10" t="s">
+      <c r="C10" s="4"/>
+      <c r="D10" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="F10" t="s">
-        <v>8</v>
-      </c>
-      <c r="G10" t="s">
-        <v>8</v>
-      </c>
-      <c r="H10">
-        <v>5</v>
-      </c>
-      <c r="J10" t="s">
+      <c r="E10" s="4"/>
+      <c r="F10" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H10" s="4">
+        <v>5</v>
+      </c>
+      <c r="K10" s="4" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A11">
+      <c r="A11" s="4">
         <v>17</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D11" t="s">
+      <c r="C11" s="4"/>
+      <c r="D11" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="F11" t="s">
-        <v>8</v>
-      </c>
-      <c r="G11" t="s">
-        <v>8</v>
-      </c>
-      <c r="H11">
+      <c r="E11" s="4"/>
+      <c r="F11" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H11" s="4">
         <v>3.6</v>
       </c>
+      <c r="L11" t="s">
+        <v>126</v>
+      </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A12">
+      <c r="A12" s="4">
         <v>18</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="4" t="s">
         <v>21</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="F12" t="s">
-        <v>8</v>
-      </c>
-      <c r="G12" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="H12">
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H12" s="4">
         <v>3.6</v>
       </c>
-      <c r="J12" s="2" t="s">
-        <v>91</v>
+      <c r="J12" s="2"/>
+      <c r="L12" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A13">
+      <c r="A13" s="4">
         <v>19</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C13" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="F13" t="s">
-        <v>8</v>
-      </c>
-      <c r="G13" t="s">
-        <v>8</v>
-      </c>
-      <c r="H13">
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H13" s="4">
         <v>3.6</v>
       </c>
-      <c r="J13" s="2" t="s">
-        <v>92</v>
-      </c>
+      <c r="J13" s="2"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A14">
+      <c r="A14" s="4">
         <v>20</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C14" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="F14" t="s">
-        <v>8</v>
-      </c>
-      <c r="G14" t="s">
-        <v>8</v>
-      </c>
-      <c r="H14">
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H14" s="4">
         <v>3.6</v>
       </c>
-      <c r="J14" s="2" t="s">
-        <v>93</v>
-      </c>
+      <c r="J14" s="2"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A15">
+      <c r="A15" s="4">
         <v>21</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C15" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="F15" t="s">
-        <v>8</v>
-      </c>
-      <c r="G15" t="s">
-        <v>8</v>
-      </c>
-      <c r="H15">
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H15" s="4">
         <v>3.6</v>
       </c>
-      <c r="J15" s="2" t="s">
-        <v>94</v>
-      </c>
+      <c r="J15" s="2"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A16">
+      <c r="A16" s="4">
         <v>22</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="D16" t="s">
+      <c r="C16" s="4"/>
+      <c r="D16" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="F16" t="s">
-        <v>8</v>
-      </c>
-      <c r="G16" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="H16">
-        <v>5</v>
-      </c>
-      <c r="J16" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A17">
+      <c r="E16" s="4"/>
+      <c r="F16" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G16" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H16" s="4">
+        <v>5</v>
+      </c>
+      <c r="K16" s="2" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A17" s="4">
         <v>23</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="D17" t="s">
+      <c r="C17" s="4"/>
+      <c r="D17" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="F17" t="s">
-        <v>8</v>
-      </c>
-      <c r="G17" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="H17">
+      <c r="E17" s="4"/>
+      <c r="F17" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G17" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H17" s="4">
         <v>3.6</v>
       </c>
-      <c r="J17" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A18">
+      <c r="K17" s="2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A18" s="4">
         <v>24</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="F18" t="s">
-        <v>8</v>
-      </c>
-      <c r="G18" t="s">
-        <v>8</v>
-      </c>
-      <c r="H18">
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G18" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H18" s="4">
         <v>3.6</v>
       </c>
-      <c r="K18" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A19">
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A19" s="4">
         <v>25</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="F19" t="s">
-        <v>8</v>
-      </c>
-      <c r="G19" t="s">
-        <v>8</v>
-      </c>
-      <c r="H19">
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G19" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H19" s="4">
         <v>3.6</v>
       </c>
-      <c r="K19" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A20">
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A20" s="4">
         <v>26</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="F20" t="s">
-        <v>8</v>
-      </c>
-      <c r="G20" t="s">
-        <v>8</v>
-      </c>
-      <c r="H20">
+      <c r="C20" s="4"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G20" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H20" s="4">
         <v>3.6</v>
       </c>
-      <c r="K20" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A21">
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A21" s="4">
         <v>30</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="D21" t="s">
+      <c r="C21" s="4"/>
+      <c r="D21" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="G21" t="s">
-        <v>8</v>
-      </c>
-      <c r="H21">
+      <c r="E21" s="4"/>
+      <c r="F21" s="4"/>
+      <c r="G21" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H21" s="4">
         <v>3.6</v>
       </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A22">
+      <c r="L21" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A22" s="4">
         <v>33</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="D22" t="s">
+      <c r="C22" s="4"/>
+      <c r="D22" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="F22" t="s">
-        <v>8</v>
-      </c>
-      <c r="G22" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="H22">
+      <c r="E22" s="4"/>
+      <c r="F22" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G22" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H22" s="4">
         <v>3.6</v>
       </c>
-      <c r="J22" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A23">
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A23" s="4">
         <v>34</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="4" t="s">
         <v>40</v>
       </c>
       <c r="C23" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="E23" t="s">
+      <c r="D23" s="4"/>
+      <c r="E23" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="F23" t="s">
-        <v>8</v>
-      </c>
-      <c r="G23" t="s">
-        <v>8</v>
-      </c>
-      <c r="H23">
+      <c r="F23" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G23" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H23" s="4">
         <v>3.6</v>
       </c>
-      <c r="J23" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A24">
+      <c r="J23" s="4" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A24" s="4">
         <v>35</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="4" t="s">
         <v>44</v>
       </c>
       <c r="C24" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="E24" t="s">
+      <c r="D24" s="4"/>
+      <c r="E24" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="F24" t="s">
-        <v>8</v>
-      </c>
-      <c r="G24" t="s">
-        <v>8</v>
-      </c>
-      <c r="H24">
+      <c r="F24" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G24" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H24" s="4">
         <v>3.6</v>
       </c>
-      <c r="J24" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A25">
+      <c r="J24" s="4" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A25" s="4">
         <v>36</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" s="4" t="s">
         <v>47</v>
       </c>
       <c r="C25" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="F25" t="s">
-        <v>8</v>
-      </c>
-      <c r="G25" t="s">
-        <v>8</v>
-      </c>
-      <c r="H25">
+      <c r="D25" s="4"/>
+      <c r="E25" s="4"/>
+      <c r="F25" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G25" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H25" s="4">
         <v>3.6</v>
       </c>
       <c r="J25" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A26">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A26" s="4">
         <v>37</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26" s="4" t="s">
         <v>49</v>
       </c>
       <c r="C26" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="F26" t="s">
-        <v>8</v>
-      </c>
-      <c r="G26" t="s">
-        <v>8</v>
-      </c>
-      <c r="H26">
+      <c r="D26" s="4"/>
+      <c r="E26" s="4"/>
+      <c r="F26" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G26" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H26" s="4">
         <v>3.6</v>
       </c>
       <c r="J26" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A27">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A27" s="4">
         <v>38</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B27" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="F27" t="s">
-        <v>8</v>
-      </c>
-      <c r="G27" t="s">
-        <v>8</v>
-      </c>
-      <c r="H27">
-        <v>5</v>
-      </c>
-      <c r="K27" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A28">
+      <c r="C27" s="4"/>
+      <c r="D27" s="4"/>
+      <c r="E27" s="4"/>
+      <c r="F27" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G27" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H27" s="4">
+        <v>5</v>
+      </c>
+      <c r="L27" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A28" s="4">
         <v>39</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B28" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="F28" t="s">
-        <v>8</v>
-      </c>
-      <c r="G28" t="s">
-        <v>8</v>
-      </c>
-      <c r="H28">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A29">
+      <c r="C28" s="4"/>
+      <c r="D28" s="4"/>
+      <c r="E28" s="4"/>
+      <c r="F28" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G28" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H28" s="4">
+        <v>5</v>
+      </c>
+      <c r="K28" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A29" s="4">
         <v>40</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B29" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="F29" t="s">
-        <v>8</v>
-      </c>
-      <c r="G29" t="s">
-        <v>8</v>
-      </c>
-      <c r="H29">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A30">
+      <c r="C29" s="4"/>
+      <c r="D29" s="4"/>
+      <c r="E29" s="4"/>
+      <c r="F29" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G29" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H29" s="4">
+        <v>5</v>
+      </c>
+      <c r="L29" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A30" s="4">
         <v>41</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B30" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="F30" t="s">
-        <v>8</v>
-      </c>
-      <c r="G30" t="s">
-        <v>8</v>
-      </c>
-      <c r="H30">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A31">
+      <c r="C30" s="4"/>
+      <c r="D30" s="4"/>
+      <c r="E30" s="4"/>
+      <c r="F30" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G30" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H30" s="4">
+        <v>5</v>
+      </c>
+      <c r="K30" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A31" s="4">
         <v>42</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B31" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="E31" t="s">
+      <c r="C31" s="4"/>
+      <c r="D31" s="4"/>
+      <c r="E31" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="F31" t="s">
-        <v>8</v>
-      </c>
-      <c r="G31" t="s">
-        <v>8</v>
-      </c>
-      <c r="H31">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A32">
+      <c r="F31" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G31" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H31" s="4">
+        <v>5</v>
+      </c>
+      <c r="L31" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A32" s="4">
         <v>43</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B32" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="F32" t="s">
-        <v>8</v>
-      </c>
-      <c r="G32" t="s">
-        <v>8</v>
-      </c>
-      <c r="H32">
-        <v>5</v>
-      </c>
-      <c r="K32" t="s">
-        <v>119</v>
+      <c r="C32" s="4"/>
+      <c r="D32" s="4"/>
+      <c r="E32" s="4"/>
+      <c r="F32" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G32" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H32" s="4">
+        <v>5</v>
+      </c>
+      <c r="L32" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A33">
+      <c r="A33" s="4">
         <v>44</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B33" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C33" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="D33" t="s">
+      <c r="D33" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="G33" t="s">
-        <v>8</v>
-      </c>
-      <c r="H33">
-        <v>5</v>
+      <c r="E33" s="4"/>
+      <c r="F33" s="4"/>
+      <c r="G33" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H33" s="4">
+        <v>5</v>
+      </c>
+      <c r="K33" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A34">
+      <c r="A34" s="4">
         <v>45</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B34" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C34" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="E34" t="s">
+      <c r="D34" s="4"/>
+      <c r="E34" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="G34" t="s">
-        <v>8</v>
-      </c>
-      <c r="H34">
-        <v>5</v>
+      <c r="F34" s="4"/>
+      <c r="G34" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H34" s="4">
+        <v>5</v>
+      </c>
+      <c r="J34" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A35">
+      <c r="A35" s="4">
         <v>46</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B35" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="E35" t="s">
+      <c r="C35" s="4"/>
+      <c r="D35" s="4"/>
+      <c r="E35" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="G35" t="s">
-        <v>8</v>
-      </c>
-      <c r="H35">
-        <v>5</v>
+      <c r="F35" s="4"/>
+      <c r="G35" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H35" s="4">
+        <v>5</v>
+      </c>
+      <c r="J35" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A36">
+      <c r="A36" s="4">
         <v>49</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B36" s="4" t="s">
         <v>63</v>
       </c>
       <c r="C36" s="5" t="s">
@@ -1571,18 +1670,15 @@
       <c r="E36" s="5"/>
       <c r="F36" s="5"/>
       <c r="G36" s="5"/>
-      <c r="H36">
-        <v>5</v>
-      </c>
-      <c r="J36" t="s">
-        <v>64</v>
+      <c r="H36" s="4">
+        <v>5</v>
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A37">
+      <c r="A37" s="4">
         <v>50</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B37" s="4" t="s">
         <v>65</v>
       </c>
       <c r="C37" s="5" t="s">
@@ -1592,189 +1688,194 @@
       <c r="E37" s="5"/>
       <c r="F37" s="5"/>
       <c r="G37" s="5"/>
-      <c r="H37">
-        <v>5</v>
-      </c>
-      <c r="J37" t="s">
-        <v>66</v>
+      <c r="H37" s="4">
+        <v>5</v>
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A38">
+      <c r="A38" s="4">
         <v>51</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B38" s="4" t="s">
         <v>67</v>
       </c>
       <c r="C38" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D38" t="s">
+      <c r="D38" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E38" t="s">
+      <c r="E38" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="G38" t="s">
-        <v>8</v>
-      </c>
-      <c r="H38">
-        <v>5</v>
-      </c>
-      <c r="L38" t="s">
-        <v>124</v>
+      <c r="F38" s="4"/>
+      <c r="G38" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H38" s="4">
+        <v>5</v>
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A39">
+      <c r="A39" s="4">
         <v>52</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B39" s="4" t="s">
         <v>69</v>
       </c>
       <c r="C39" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="D39" t="s">
+      <c r="D39" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="G39" t="s">
-        <v>8</v>
-      </c>
-      <c r="H39">
-        <v>5</v>
-      </c>
-      <c r="L39" t="s">
-        <v>124</v>
+      <c r="E39" s="4"/>
+      <c r="F39" s="4"/>
+      <c r="G39" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H39" s="4">
+        <v>5</v>
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A40">
+      <c r="A40" s="4">
         <v>53</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B40" s="4" t="s">
         <v>72</v>
       </c>
       <c r="C40" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="D40" t="s">
+      <c r="D40" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="G40" t="s">
-        <v>8</v>
-      </c>
-      <c r="H40">
-        <v>5</v>
+      <c r="E40" s="4"/>
+      <c r="F40" s="4"/>
+      <c r="G40" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H40" s="4">
+        <v>5</v>
+      </c>
+      <c r="L40" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A41">
+      <c r="A41" s="4">
         <v>54</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B41" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="C41" t="s">
+      <c r="C41" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="D41" s="3" t="s">
+      <c r="D41" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="G41" t="s">
-        <v>8</v>
-      </c>
-      <c r="H41">
-        <v>5</v>
-      </c>
-      <c r="J41" t="s">
-        <v>97</v>
+      <c r="E41" s="4"/>
+      <c r="F41" s="4"/>
+      <c r="G41" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H41" s="4">
+        <v>5</v>
+      </c>
+      <c r="L41" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A42">
+      <c r="A42" s="4">
         <v>55</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B42" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="D42" s="3" t="s">
+      <c r="C42" s="4"/>
+      <c r="D42" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="G42" t="s">
-        <v>8</v>
-      </c>
-      <c r="H42">
-        <v>5</v>
-      </c>
-      <c r="J42" t="s">
-        <v>98</v>
+      <c r="E42" s="4"/>
+      <c r="F42" s="4"/>
+      <c r="G42" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H42" s="4">
+        <v>5</v>
+      </c>
+      <c r="L42" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A43">
+      <c r="A43" s="4">
         <v>56</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B43" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="C43" s="6" t="s">
+      <c r="C43" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="D43" s="6"/>
-      <c r="E43" s="6"/>
-      <c r="F43" s="6"/>
-      <c r="G43" s="6"/>
-      <c r="H43">
-        <v>5</v>
-      </c>
-      <c r="J43" t="s">
-        <v>81</v>
+      <c r="D43" s="5"/>
+      <c r="E43" s="5"/>
+      <c r="F43" s="5"/>
+      <c r="G43" s="5"/>
+      <c r="H43" s="4">
+        <v>5</v>
       </c>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A44">
+      <c r="A44" s="4">
         <v>57</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B44" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="C44" t="s">
+      <c r="C44" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="D44" t="s">
+      <c r="D44" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E44" t="s">
+      <c r="E44" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="G44" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="H44">
-        <v>5</v>
-      </c>
-      <c r="J44" s="4" t="s">
-        <v>101</v>
+      <c r="F44" s="4"/>
+      <c r="G44" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H44" s="4">
+        <v>5</v>
+      </c>
+      <c r="J44" s="4"/>
+      <c r="L44" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A45">
+      <c r="A45" s="4">
         <v>58</v>
       </c>
-      <c r="B45" t="s">
+      <c r="B45" s="4" t="s">
         <v>84</v>
       </c>
       <c r="C45" s="4" t="s">
         <v>85</v>
       </c>
+      <c r="D45" s="4"/>
       <c r="E45" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="G45" t="s">
-        <v>8</v>
-      </c>
-      <c r="H45">
+      <c r="F45" s="4"/>
+      <c r="G45" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H45" s="4">
         <v>5</v>
       </c>
       <c r="J45" t="s">
@@ -1782,22 +1883,24 @@
       </c>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A46">
+      <c r="A46" s="4">
         <v>59</v>
       </c>
-      <c r="B46" t="s">
+      <c r="B46" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="D46" t="s">
+      <c r="C46" s="4"/>
+      <c r="D46" s="4" t="s">
         <v>30</v>
       </c>
       <c r="E46" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="G46" t="s">
-        <v>8</v>
-      </c>
-      <c r="H46">
+      <c r="F46" s="4"/>
+      <c r="G46" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H46" s="4">
         <v>5</v>
       </c>
       <c r="J46" t="s">
@@ -1805,69 +1908,76 @@
       </c>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A47">
+      <c r="A47" s="4">
         <v>60</v>
       </c>
-      <c r="B47" t="s">
+      <c r="B47" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="D47" t="s">
+      <c r="C47" s="4"/>
+      <c r="D47" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="G47" t="s">
-        <v>8</v>
-      </c>
-      <c r="H47">
+      <c r="E47" s="4"/>
+      <c r="F47" s="4"/>
+      <c r="G47" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H47" s="4">
         <v>5</v>
       </c>
       <c r="L47" t="s">
-        <v>122</v>
+        <v>110</v>
       </c>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A48">
+      <c r="A48" s="4">
         <v>61</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B48" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="D48" t="s">
+      <c r="C48" s="4"/>
+      <c r="D48" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="E48" s="3" t="s">
+      <c r="E48" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="G48" t="s">
-        <v>8</v>
-      </c>
-      <c r="H48">
-        <v>5</v>
-      </c>
-      <c r="J48" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A49">
+      <c r="F48" s="4"/>
+      <c r="G48" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H48" s="4">
+        <v>5</v>
+      </c>
+      <c r="L48" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A49" s="4">
         <v>62</v>
       </c>
-      <c r="B49" t="s">
+      <c r="B49" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="D49" t="s">
+      <c r="C49" s="4"/>
+      <c r="D49" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="E49" s="3" t="s">
+      <c r="E49" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="G49" t="s">
-        <v>8</v>
-      </c>
-      <c r="H49">
-        <v>5</v>
-      </c>
-      <c r="J49" t="s">
-        <v>103</v>
+      <c r="F49" s="4"/>
+      <c r="G49" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H49" s="4">
+        <v>5</v>
+      </c>
+      <c r="L49" t="s">
+        <v>115</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
working to finalize boards now, NAV needs rework and logo/LED/test placement as well as outline needs to be homogenized across boards
</commit_message>
<xml_diff>
--- a/HYDRA_V4_POWER/STM32G473RET6_PINOUT.xlsx
+++ b/HYDRA_V4_POWER/STM32G473RET6_PINOUT.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\se097192\Documents\0_PERSONAL\HYDRA\HYDRA_V4_POWER\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Trololololol\Documents\Projects\HYDRA\HYDRA_V4_POWER\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04370D79-7979-4F57-9489-FDE56ADEFD8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2F8A5F0-0A33-46E6-819B-E2970A23BA1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6B9885FF-AF60-4EEC-BBBC-D143F7D9FDBE}"/>
+    <workbookView xWindow="-28920" yWindow="2490" windowWidth="29040" windowHeight="16440" xr2:uid="{6B9885FF-AF60-4EEC-BBBC-D143F7D9FDBE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="130">
   <si>
     <t>SPI</t>
   </si>
@@ -420,6 +420,12 @@
   </si>
   <si>
     <t>MCU_G_LED</t>
+  </si>
+  <si>
+    <t>EMAG</t>
+  </si>
+  <si>
+    <t>FORCE ON</t>
   </si>
 </sst>
 </file>
@@ -467,15 +473,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -815,33 +816,33 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71B6B797-796C-44D6-BE9C-10AF3EFF403F}">
   <dimension ref="A1:L49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="L11" sqref="C11:L11"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="L40" sqref="L40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="4.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5.44140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.44140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.109375" style="1"/>
-    <col min="10" max="10" width="18.44140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="19.88671875" customWidth="1"/>
+    <col min="1" max="1" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.140625" style="1"/>
+    <col min="10" max="10" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="J1" s="6" t="s">
+    <row r="1" spans="1:12" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J1" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="K1" s="6"/>
-      <c r="L1" s="6"/>
-    </row>
-    <row r="2" spans="1:12" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+    </row>
+    <row r="2" spans="1:12" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -876,1104 +877,1003 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A3" s="4">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="H3" s="4">
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H3">
         <v>5</v>
       </c>
       <c r="K3" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A4" s="4">
-        <v>8</v>
-      </c>
-      <c r="B4" s="4" t="s">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4" t="s">
+      <c r="D4" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="H4" s="4">
+      <c r="F4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H4">
         <v>5</v>
       </c>
       <c r="K4" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A5" s="4">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5">
         <v>9</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4" t="s">
+      <c r="D5" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="H5" s="4">
+      <c r="F5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G5" t="s">
+        <v>8</v>
+      </c>
+      <c r="H5">
         <v>3.6</v>
       </c>
-      <c r="K5" s="4" t="s">
+      <c r="K5" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A6" s="4">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6">
         <v>10</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="H6" s="4">
-        <v>5</v>
-      </c>
-      <c r="K6" s="4" t="s">
+      <c r="F6" t="s">
+        <v>8</v>
+      </c>
+      <c r="G6" t="s">
+        <v>8</v>
+      </c>
+      <c r="H6">
+        <v>5</v>
+      </c>
+      <c r="K6" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A7" s="4">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7">
         <v>11</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="G7" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="H7" s="4">
+      <c r="F7" t="s">
+        <v>8</v>
+      </c>
+      <c r="G7" t="s">
+        <v>8</v>
+      </c>
+      <c r="H7">
         <v>3.6</v>
       </c>
-      <c r="K7" s="4" t="s">
+      <c r="K7" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A8" s="4">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8">
         <v>12</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="G8" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="H8" s="4">
+      <c r="F8" t="s">
+        <v>8</v>
+      </c>
+      <c r="G8" t="s">
+        <v>8</v>
+      </c>
+      <c r="H8">
         <v>3.6</v>
       </c>
-      <c r="K8" s="4" t="s">
+      <c r="K8" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A9" s="4">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9">
         <v>13</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="G9" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="H9" s="4">
+      <c r="F9" t="s">
+        <v>8</v>
+      </c>
+      <c r="G9" t="s">
+        <v>8</v>
+      </c>
+      <c r="H9">
         <v>3.6</v>
       </c>
-      <c r="K9" s="4" t="s">
+      <c r="K9" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A10" s="4">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10">
         <v>14</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4" t="s">
+      <c r="D10" t="s">
         <v>18</v>
       </c>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="G10" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="H10" s="4">
-        <v>5</v>
-      </c>
-      <c r="K10" s="4" t="s">
+      <c r="F10" t="s">
+        <v>8</v>
+      </c>
+      <c r="G10" t="s">
+        <v>8</v>
+      </c>
+      <c r="H10">
+        <v>5</v>
+      </c>
+      <c r="K10" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A11" s="4">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11">
         <v>17</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" t="s">
         <v>19</v>
       </c>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4" t="s">
+      <c r="D11" t="s">
         <v>20</v>
       </c>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="G11" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="H11" s="4">
+      <c r="F11" t="s">
+        <v>8</v>
+      </c>
+      <c r="G11" t="s">
+        <v>8</v>
+      </c>
+      <c r="H11">
         <v>3.6</v>
       </c>
       <c r="L11" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A12" s="4">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12">
         <v>18</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" t="s">
         <v>21</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C12" t="s">
         <v>22</v>
       </c>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="G12" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="H12" s="4">
+      <c r="F12" t="s">
+        <v>8</v>
+      </c>
+      <c r="G12" t="s">
+        <v>8</v>
+      </c>
+      <c r="H12">
         <v>3.6</v>
       </c>
-      <c r="J12" s="2"/>
       <c r="L12" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A13" s="4">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13">
         <v>19</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="B13" t="s">
         <v>23</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="C13" t="s">
         <v>26</v>
       </c>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="G13" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="H13" s="4">
+      <c r="F13" t="s">
+        <v>8</v>
+      </c>
+      <c r="G13" t="s">
+        <v>8</v>
+      </c>
+      <c r="H13">
         <v>3.6</v>
       </c>
-      <c r="J13" s="2"/>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A14" s="4">
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14">
         <v>20</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B14" t="s">
         <v>25</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="C14" t="s">
         <v>27</v>
       </c>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="G14" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="H14" s="4">
+      <c r="F14" t="s">
+        <v>8</v>
+      </c>
+      <c r="G14" t="s">
+        <v>8</v>
+      </c>
+      <c r="H14">
         <v>3.6</v>
       </c>
-      <c r="J14" s="2"/>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A15" s="4">
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15">
         <v>21</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="B15" t="s">
         <v>24</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="C15" t="s">
         <v>28</v>
       </c>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="G15" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="H15" s="4">
+      <c r="F15" t="s">
+        <v>8</v>
+      </c>
+      <c r="G15" t="s">
+        <v>8</v>
+      </c>
+      <c r="H15">
         <v>3.6</v>
       </c>
-      <c r="J15" s="2"/>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A16" s="4">
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16">
         <v>22</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="B16" t="s">
         <v>29</v>
       </c>
-      <c r="C16" s="4"/>
-      <c r="D16" s="4" t="s">
+      <c r="D16" t="s">
         <v>30</v>
       </c>
-      <c r="E16" s="4"/>
-      <c r="F16" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="G16" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="H16" s="4">
-        <v>5</v>
-      </c>
-      <c r="K16" s="2" t="s">
+      <c r="F16" t="s">
+        <v>8</v>
+      </c>
+      <c r="G16" t="s">
+        <v>8</v>
+      </c>
+      <c r="H16">
+        <v>5</v>
+      </c>
+      <c r="K16" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A17" s="4">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17">
         <v>23</v>
       </c>
-      <c r="B17" s="4" t="s">
+      <c r="B17" t="s">
         <v>31</v>
       </c>
-      <c r="C17" s="4"/>
-      <c r="D17" s="4" t="s">
+      <c r="D17" t="s">
         <v>32</v>
       </c>
-      <c r="E17" s="4"/>
-      <c r="F17" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="G17" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="H17" s="4">
+      <c r="F17" t="s">
+        <v>8</v>
+      </c>
+      <c r="G17" t="s">
+        <v>8</v>
+      </c>
+      <c r="H17">
         <v>3.6</v>
       </c>
-      <c r="K17" s="2" t="s">
+      <c r="K17" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A18" s="4">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A18">
         <v>24</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="B18" t="s">
         <v>33</v>
       </c>
-      <c r="C18" s="4"/>
-      <c r="D18" s="4"/>
-      <c r="E18" s="4"/>
-      <c r="F18" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="G18" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="H18" s="4">
+      <c r="F18" t="s">
+        <v>8</v>
+      </c>
+      <c r="G18" t="s">
+        <v>8</v>
+      </c>
+      <c r="H18">
         <v>3.6</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A19" s="4">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A19">
         <v>25</v>
       </c>
-      <c r="B19" s="4" t="s">
+      <c r="B19" t="s">
         <v>34</v>
       </c>
-      <c r="C19" s="4"/>
-      <c r="D19" s="4"/>
-      <c r="E19" s="4"/>
-      <c r="F19" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="G19" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="H19" s="4">
+      <c r="F19" t="s">
+        <v>8</v>
+      </c>
+      <c r="G19" t="s">
+        <v>8</v>
+      </c>
+      <c r="H19">
         <v>3.6</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A20" s="4">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A20">
         <v>26</v>
       </c>
-      <c r="B20" s="4" t="s">
+      <c r="B20" t="s">
         <v>35</v>
       </c>
-      <c r="C20" s="4"/>
-      <c r="D20" s="4"/>
-      <c r="E20" s="4"/>
-      <c r="F20" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="G20" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="H20" s="4">
+      <c r="F20" t="s">
+        <v>8</v>
+      </c>
+      <c r="G20" t="s">
+        <v>8</v>
+      </c>
+      <c r="H20">
         <v>3.6</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A21" s="4">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A21">
         <v>30</v>
       </c>
-      <c r="B21" s="4" t="s">
+      <c r="B21" t="s">
         <v>36</v>
       </c>
-      <c r="C21" s="4"/>
-      <c r="D21" s="4" t="s">
+      <c r="D21" t="s">
         <v>37</v>
       </c>
-      <c r="E21" s="4"/>
-      <c r="F21" s="4"/>
-      <c r="G21" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="H21" s="4">
+      <c r="G21" t="s">
+        <v>8</v>
+      </c>
+      <c r="H21">
         <v>3.6</v>
       </c>
       <c r="L21" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A22" s="4">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A22">
         <v>33</v>
       </c>
-      <c r="B22" s="4" t="s">
+      <c r="B22" t="s">
         <v>38</v>
       </c>
-      <c r="C22" s="4"/>
-      <c r="D22" s="4" t="s">
+      <c r="D22" t="s">
         <v>39</v>
       </c>
-      <c r="E22" s="4"/>
-      <c r="F22" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="G22" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="H22" s="4">
+      <c r="F22" t="s">
+        <v>8</v>
+      </c>
+      <c r="G22" t="s">
+        <v>8</v>
+      </c>
+      <c r="H22">
         <v>3.6</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A23" s="4">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A23">
         <v>34</v>
       </c>
-      <c r="B23" s="4" t="s">
+      <c r="B23" t="s">
         <v>40</v>
       </c>
-      <c r="C23" s="3" t="s">
+      <c r="C23" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="D23" s="4"/>
-      <c r="E23" s="4" t="s">
+      <c r="E23" t="s">
         <v>43</v>
       </c>
-      <c r="F23" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="G23" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="H23" s="4">
+      <c r="F23" t="s">
+        <v>8</v>
+      </c>
+      <c r="G23" t="s">
+        <v>8</v>
+      </c>
+      <c r="H23">
         <v>3.6</v>
       </c>
-      <c r="J23" s="4" t="s">
+      <c r="J23" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A24" s="4">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A24">
         <v>35</v>
       </c>
-      <c r="B24" s="4" t="s">
+      <c r="B24" t="s">
         <v>44</v>
       </c>
-      <c r="C24" s="3" t="s">
+      <c r="C24" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="D24" s="4"/>
-      <c r="E24" s="4" t="s">
+      <c r="E24" t="s">
         <v>46</v>
       </c>
-      <c r="F24" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="G24" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="H24" s="4">
+      <c r="F24" t="s">
+        <v>8</v>
+      </c>
+      <c r="G24" t="s">
+        <v>8</v>
+      </c>
+      <c r="H24">
         <v>3.6</v>
       </c>
-      <c r="J24" s="4" t="s">
+      <c r="J24" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A25" s="4">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A25">
         <v>36</v>
       </c>
-      <c r="B25" s="4" t="s">
+      <c r="B25" t="s">
         <v>47</v>
       </c>
-      <c r="C25" s="3" t="s">
+      <c r="C25" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="D25" s="4"/>
-      <c r="E25" s="4"/>
-      <c r="F25" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="G25" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="H25" s="4">
+      <c r="F25" t="s">
+        <v>8</v>
+      </c>
+      <c r="G25" t="s">
+        <v>8</v>
+      </c>
+      <c r="H25">
         <v>3.6</v>
       </c>
       <c r="J25" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A26" s="4">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A26">
         <v>37</v>
       </c>
-      <c r="B26" s="4" t="s">
+      <c r="B26" t="s">
         <v>49</v>
       </c>
-      <c r="C26" s="3" t="s">
+      <c r="C26" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="D26" s="4"/>
-      <c r="E26" s="4"/>
-      <c r="F26" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="G26" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="H26" s="4">
+      <c r="F26" t="s">
+        <v>8</v>
+      </c>
+      <c r="G26" t="s">
+        <v>8</v>
+      </c>
+      <c r="H26">
         <v>3.6</v>
       </c>
       <c r="J26" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A27" s="4">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A27">
         <v>38</v>
       </c>
-      <c r="B27" s="4" t="s">
+      <c r="B27" t="s">
         <v>51</v>
       </c>
-      <c r="C27" s="4"/>
-      <c r="D27" s="4"/>
-      <c r="E27" s="4"/>
-      <c r="F27" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="G27" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="H27" s="4">
+      <c r="F27" t="s">
+        <v>8</v>
+      </c>
+      <c r="G27" t="s">
+        <v>8</v>
+      </c>
+      <c r="H27">
         <v>5</v>
       </c>
       <c r="L27" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A28" s="4">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A28">
         <v>39</v>
       </c>
-      <c r="B28" s="4" t="s">
+      <c r="B28" t="s">
         <v>52</v>
       </c>
-      <c r="C28" s="4"/>
-      <c r="D28" s="4"/>
-      <c r="E28" s="4"/>
-      <c r="F28" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="G28" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="H28" s="4">
+      <c r="F28" t="s">
+        <v>8</v>
+      </c>
+      <c r="G28" t="s">
+        <v>8</v>
+      </c>
+      <c r="H28">
         <v>5</v>
       </c>
       <c r="K28" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A29" s="4">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A29">
         <v>40</v>
       </c>
-      <c r="B29" s="4" t="s">
+      <c r="B29" t="s">
         <v>53</v>
       </c>
-      <c r="C29" s="4"/>
-      <c r="D29" s="4"/>
-      <c r="E29" s="4"/>
-      <c r="F29" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="G29" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="H29" s="4">
+      <c r="F29" t="s">
+        <v>8</v>
+      </c>
+      <c r="G29" t="s">
+        <v>8</v>
+      </c>
+      <c r="H29">
         <v>5</v>
       </c>
       <c r="L29" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A30" s="4">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A30">
         <v>41</v>
       </c>
-      <c r="B30" s="4" t="s">
+      <c r="B30" t="s">
         <v>54</v>
       </c>
-      <c r="C30" s="4"/>
-      <c r="D30" s="4"/>
-      <c r="E30" s="4"/>
-      <c r="F30" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="G30" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="H30" s="4">
+      <c r="F30" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G30" t="s">
+        <v>8</v>
+      </c>
+      <c r="H30">
         <v>5</v>
       </c>
       <c r="K30" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A31" s="4">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A31">
         <v>42</v>
       </c>
-      <c r="B31" s="4" t="s">
+      <c r="B31" t="s">
         <v>55</v>
       </c>
-      <c r="C31" s="4"/>
-      <c r="D31" s="4"/>
-      <c r="E31" s="4" t="s">
+      <c r="E31" t="s">
         <v>56</v>
       </c>
-      <c r="F31" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="G31" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="H31" s="4">
+      <c r="F31" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G31" t="s">
+        <v>8</v>
+      </c>
+      <c r="H31">
         <v>5</v>
       </c>
       <c r="L31" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A32" s="4">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A32">
         <v>43</v>
       </c>
-      <c r="B32" s="4" t="s">
+      <c r="B32" t="s">
         <v>57</v>
       </c>
-      <c r="C32" s="4"/>
-      <c r="D32" s="4"/>
-      <c r="E32" s="4"/>
-      <c r="F32" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="G32" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="H32" s="4">
+      <c r="F32" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G32" t="s">
+        <v>8</v>
+      </c>
+      <c r="H32">
         <v>5</v>
       </c>
       <c r="L32" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A33" s="4">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A33">
         <v>44</v>
       </c>
-      <c r="B33" s="4" t="s">
+      <c r="B33" t="s">
         <v>58</v>
       </c>
-      <c r="C33" s="4" t="s">
+      <c r="C33" t="s">
         <v>48</v>
       </c>
-      <c r="D33" s="4" t="s">
+      <c r="D33" t="s">
         <v>32</v>
       </c>
-      <c r="E33" s="4"/>
-      <c r="F33" s="4"/>
-      <c r="G33" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="H33" s="4">
+      <c r="G33" t="s">
+        <v>8</v>
+      </c>
+      <c r="H33">
         <v>5</v>
       </c>
       <c r="K33" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A34" s="4">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A34">
         <v>45</v>
       </c>
-      <c r="B34" s="4" t="s">
+      <c r="B34" t="s">
         <v>59</v>
       </c>
-      <c r="C34" s="4" t="s">
+      <c r="C34" t="s">
         <v>50</v>
       </c>
-      <c r="D34" s="4"/>
-      <c r="E34" s="3" t="s">
+      <c r="E34" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="F34" s="4"/>
-      <c r="G34" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="H34" s="4">
+      <c r="G34" t="s">
+        <v>8</v>
+      </c>
+      <c r="H34">
         <v>5</v>
       </c>
       <c r="J34" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A35" s="4">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A35">
         <v>46</v>
       </c>
-      <c r="B35" s="4" t="s">
+      <c r="B35" t="s">
         <v>61</v>
       </c>
-      <c r="C35" s="4"/>
-      <c r="D35" s="4"/>
-      <c r="E35" s="3" t="s">
+      <c r="E35" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="F35" s="4"/>
-      <c r="G35" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="H35" s="4">
+      <c r="G35" t="s">
+        <v>8</v>
+      </c>
+      <c r="H35">
         <v>5</v>
       </c>
       <c r="J35" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A36" s="4">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A36">
         <v>49</v>
       </c>
-      <c r="B36" s="4" t="s">
+      <c r="B36" t="s">
         <v>63</v>
       </c>
-      <c r="C36" s="5" t="s">
+      <c r="C36" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="D36" s="5"/>
-      <c r="E36" s="5"/>
-      <c r="F36" s="5"/>
-      <c r="G36" s="5"/>
-      <c r="H36" s="4">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A37" s="4">
+      <c r="D36" s="3"/>
+      <c r="E36" s="3"/>
+      <c r="F36" s="3"/>
+      <c r="G36" s="3"/>
+      <c r="H36">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A37">
         <v>50</v>
       </c>
-      <c r="B37" s="4" t="s">
+      <c r="B37" t="s">
         <v>65</v>
       </c>
-      <c r="C37" s="5" t="s">
+      <c r="C37" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="D37" s="5"/>
-      <c r="E37" s="5"/>
-      <c r="F37" s="5"/>
-      <c r="G37" s="5"/>
-      <c r="H37" s="4">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A38" s="4">
+      <c r="D37" s="3"/>
+      <c r="E37" s="3"/>
+      <c r="F37" s="3"/>
+      <c r="G37" s="3"/>
+      <c r="H37">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A38">
         <v>51</v>
       </c>
-      <c r="B38" s="4" t="s">
+      <c r="B38" t="s">
         <v>67</v>
       </c>
-      <c r="C38" s="4" t="s">
+      <c r="C38" t="s">
         <v>22</v>
       </c>
-      <c r="D38" s="4" t="s">
+      <c r="D38" t="s">
         <v>20</v>
       </c>
-      <c r="E38" s="4" t="s">
+      <c r="E38" t="s">
         <v>68</v>
       </c>
-      <c r="F38" s="4"/>
-      <c r="G38" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="H38" s="4">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A39" s="4">
+      <c r="G38" t="s">
+        <v>8</v>
+      </c>
+      <c r="H38">
+        <v>5</v>
+      </c>
+      <c r="L38" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A39">
         <v>52</v>
       </c>
-      <c r="B39" s="4" t="s">
+      <c r="B39" t="s">
         <v>69</v>
       </c>
-      <c r="C39" s="4" t="s">
+      <c r="C39" t="s">
         <v>70</v>
       </c>
-      <c r="D39" s="4" t="s">
+      <c r="D39" t="s">
         <v>71</v>
       </c>
-      <c r="E39" s="4"/>
-      <c r="F39" s="4"/>
-      <c r="G39" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="H39" s="4">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A40" s="4">
+      <c r="G39" t="s">
+        <v>8</v>
+      </c>
+      <c r="H39">
+        <v>5</v>
+      </c>
+      <c r="L39" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A40">
         <v>53</v>
       </c>
-      <c r="B40" s="4" t="s">
+      <c r="B40" t="s">
         <v>72</v>
       </c>
-      <c r="C40" s="4" t="s">
+      <c r="C40" t="s">
         <v>73</v>
       </c>
-      <c r="D40" s="4" t="s">
+      <c r="D40" t="s">
         <v>74</v>
       </c>
-      <c r="E40" s="4"/>
-      <c r="F40" s="4"/>
-      <c r="G40" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="H40" s="4">
+      <c r="G40" t="s">
+        <v>8</v>
+      </c>
+      <c r="H40">
         <v>5</v>
       </c>
       <c r="L40" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A41" s="4">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A41">
         <v>54</v>
       </c>
-      <c r="B41" s="4" t="s">
+      <c r="B41" t="s">
         <v>75</v>
       </c>
-      <c r="C41" s="4" t="s">
+      <c r="C41" t="s">
         <v>76</v>
       </c>
-      <c r="D41" s="4" t="s">
+      <c r="D41" t="s">
         <v>77</v>
       </c>
-      <c r="E41" s="4"/>
-      <c r="F41" s="4"/>
-      <c r="G41" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="H41" s="4">
+      <c r="G41" t="s">
+        <v>8</v>
+      </c>
+      <c r="H41">
         <v>5</v>
       </c>
       <c r="L41" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A42" s="4">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A42">
         <v>55</v>
       </c>
-      <c r="B42" s="4" t="s">
+      <c r="B42" t="s">
         <v>78</v>
       </c>
-      <c r="C42" s="4"/>
-      <c r="D42" s="4" t="s">
+      <c r="D42" t="s">
         <v>79</v>
       </c>
-      <c r="E42" s="4"/>
-      <c r="F42" s="4"/>
-      <c r="G42" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="H42" s="4">
+      <c r="G42" t="s">
+        <v>8</v>
+      </c>
+      <c r="H42">
         <v>5</v>
       </c>
       <c r="L42" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A43" s="4">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A43">
         <v>56</v>
       </c>
-      <c r="B43" s="4" t="s">
+      <c r="B43" t="s">
         <v>80</v>
       </c>
-      <c r="C43" s="5" t="s">
+      <c r="C43" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="D43" s="5"/>
-      <c r="E43" s="5"/>
-      <c r="F43" s="5"/>
-      <c r="G43" s="5"/>
-      <c r="H43" s="4">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A44" s="4">
+      <c r="D43" s="3"/>
+      <c r="E43" s="3"/>
+      <c r="F43" s="3"/>
+      <c r="G43" s="3"/>
+      <c r="H43">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A44">
         <v>57</v>
       </c>
-      <c r="B44" s="4" t="s">
+      <c r="B44" t="s">
         <v>82</v>
       </c>
-      <c r="C44" s="4" t="s">
+      <c r="C44" t="s">
         <v>83</v>
       </c>
-      <c r="D44" s="4" t="s">
+      <c r="D44" t="s">
         <v>20</v>
       </c>
-      <c r="E44" s="4" t="s">
+      <c r="E44" t="s">
         <v>68</v>
       </c>
-      <c r="F44" s="4"/>
-      <c r="G44" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="H44" s="4">
-        <v>5</v>
-      </c>
-      <c r="J44" s="4"/>
+      <c r="G44" t="s">
+        <v>8</v>
+      </c>
+      <c r="H44">
+        <v>5</v>
+      </c>
       <c r="L44" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A45" s="4">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A45">
         <v>58</v>
       </c>
-      <c r="B45" s="4" t="s">
+      <c r="B45" t="s">
         <v>84</v>
       </c>
-      <c r="C45" s="4" t="s">
+      <c r="C45" t="s">
         <v>85</v>
       </c>
-      <c r="D45" s="4"/>
-      <c r="E45" s="3" t="s">
+      <c r="E45" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="F45" s="4"/>
-      <c r="G45" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="H45" s="4">
+      <c r="G45" t="s">
+        <v>8</v>
+      </c>
+      <c r="H45">
         <v>5</v>
       </c>
       <c r="J45" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A46" s="4">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A46">
         <v>59</v>
       </c>
-      <c r="B46" s="4" t="s">
+      <c r="B46" t="s">
         <v>86</v>
       </c>
-      <c r="C46" s="4"/>
-      <c r="D46" s="4" t="s">
+      <c r="D46" t="s">
         <v>30</v>
       </c>
-      <c r="E46" s="3" t="s">
+      <c r="E46" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="F46" s="4"/>
-      <c r="G46" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="H46" s="4">
+      <c r="G46" t="s">
+        <v>8</v>
+      </c>
+      <c r="H46">
         <v>5</v>
       </c>
       <c r="J46" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A47" s="4">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A47">
         <v>60</v>
       </c>
-      <c r="B47" s="4" t="s">
+      <c r="B47" t="s">
         <v>87</v>
       </c>
-      <c r="C47" s="4"/>
-      <c r="D47" s="4" t="s">
+      <c r="D47" t="s">
         <v>32</v>
       </c>
-      <c r="E47" s="4"/>
-      <c r="F47" s="4"/>
-      <c r="G47" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="H47" s="4">
+      <c r="G47" t="s">
+        <v>8</v>
+      </c>
+      <c r="H47">
         <v>5</v>
       </c>
       <c r="L47" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A48" s="4">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A48">
         <v>61</v>
       </c>
-      <c r="B48" s="4" t="s">
+      <c r="B48" t="s">
         <v>88</v>
       </c>
-      <c r="C48" s="4"/>
-      <c r="D48" s="4" t="s">
+      <c r="D48" t="s">
         <v>39</v>
       </c>
-      <c r="E48" s="4" t="s">
+      <c r="E48" t="s">
         <v>60</v>
       </c>
-      <c r="F48" s="4"/>
-      <c r="G48" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="H48" s="4">
+      <c r="G48" t="s">
+        <v>8</v>
+      </c>
+      <c r="H48">
         <v>5</v>
       </c>
       <c r="L48" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A49" s="4">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A49">
         <v>62</v>
       </c>
-      <c r="B49" s="4" t="s">
+      <c r="B49" t="s">
         <v>89</v>
       </c>
-      <c r="C49" s="4"/>
-      <c r="D49" s="4" t="s">
+      <c r="D49" t="s">
         <v>37</v>
       </c>
-      <c r="E49" s="4" t="s">
+      <c r="E49" t="s">
         <v>62</v>
       </c>
-      <c r="F49" s="4"/>
-      <c r="G49" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="H49" s="4">
+      <c r="G49" t="s">
+        <v>8</v>
+      </c>
+      <c r="H49">
         <v>5</v>
       </c>
       <c r="L49" t="s">

</xml_diff>

<commit_message>
corrected power, need to wire up a pin on recovery and correct link + homogenization
</commit_message>
<xml_diff>
--- a/HYDRA_V4_POWER/STM32G473RET6_PINOUT.xlsx
+++ b/HYDRA_V4_POWER/STM32G473RET6_PINOUT.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Trololololol\Documents\Projects\HYDRA\HYDRA_V4_POWER\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\se097192\Documents\0_PERSONAL\HYDRA\HYDRA_V4_POWER\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2F8A5F0-0A33-46E6-819B-E2970A23BA1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F06372F1-FDBC-4F07-A9D8-0B151A624E9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="2490" windowWidth="29040" windowHeight="16440" xr2:uid="{6B9885FF-AF60-4EEC-BBBC-D143F7D9FDBE}"/>
+    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{6B9885FF-AF60-4EEC-BBBC-D143F7D9FDBE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -816,8 +816,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71B6B797-796C-44D6-BE9C-10AF3EFF403F}">
   <dimension ref="A1:L49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="L40" sqref="L40"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1285,6 +1285,9 @@
       <c r="H22">
         <v>3.6</v>
       </c>
+      <c r="K22" t="s">
+        <v>103</v>
+      </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23">
@@ -1419,9 +1422,6 @@
       </c>
       <c r="H28">
         <v>5</v>
-      </c>
-      <c r="K28" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">

</xml_diff>